<commit_message>
pom xml file and excel utilities
</commit_message>
<xml_diff>
--- a/testData/TestSuite1.xlsx
+++ b/testData/TestSuite1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tssum\eclipse-workspace\AutomationProject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8282477-5314-4AFB-B363-E207C56AA65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FF3759-C2B2-480E-B371-6B46CD2987CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Checkbox2FinalStatus</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Kumar</t>
   </si>
 </sst>
 </file>
@@ -370,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,7 +397,7 @@
     <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,8 +413,14 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -412,8 +430,14 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>